<commit_message>
Fix Cisco CCF v3.0 base Excel Framework
</commit_message>
<xml_diff>
--- a/tools/excel/ccf/cisco/cisco-ccf-v3.0.xlsx
+++ b/tools/excel/ccf/cisco/cisco-ccf-v3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\ccf\cisco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8626F5D7-FFC0-476C-BEE7-2168A69C0F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407E6999-A65C-4243-99D6-288CA1046D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7710" yWindow="-12960" windowWidth="18915" windowHeight="12705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="-14355" windowWidth="18915" windowHeight="12705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>type</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>depth</t>
+  </si>
+  <si>
+    <t>annotation</t>
+  </si>
+  <si>
+    <t>typical_evidence</t>
   </si>
   <si>
     <t>implementation_groups</t>
@@ -453,7 +459,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -553,11 +559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -615,17 +621,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -643,6 +651,12 @@
       </c>
       <c r="F1" t="s">
         <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>